<commit_message>
nuevo modulo de inventario ingreso kardex
</commit_message>
<xml_diff>
--- a/php/vista/TEMP/entrega de materia.xlsx
+++ b/php/vista/TEMP/entrega de materia.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <r>
       <t xml:space="preserve">HARO URRUTIA MEYBOL GISELLE </t>
@@ -60,7 +60,7 @@
         <sz val="8"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">23:51
+      <t xml:space="preserve">21:53
 </t>
     </r>
     <r>
@@ -85,7 +85,7 @@
         <sz val="8"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">01-09-2020
+      <t xml:space="preserve">07-10-2020
 </t>
     </r>
     <r>
@@ -126,7 +126,7 @@
     <t>CANT</t>
   </si>
   <si>
-    <t>Centro constos</t>
+    <t>Centro de costos</t>
   </si>
   <si>
     <t>rubro</t>
@@ -135,31 +135,55 @@
     <t>bajas o desper</t>
   </si>
   <si>
+    <t>Baja por</t>
+  </si>
+  <si>
     <t>Observaciones</t>
   </si>
   <si>
-    <t>2020-09-01</t>
-  </si>
-  <si>
-    <t>FE.01.016</t>
-  </si>
-  <si>
-    <t>BISAGRA DE PRESION</t>
-  </si>
-  <si>
-    <t>MP BLOQUE 2</t>
+    <t>2020-10-06</t>
+  </si>
+  <si>
+    <t>FE.01.002</t>
+  </si>
+  <si>
+    <t>MAT. DE FERRETERIA EN GENERAL</t>
   </si>
   <si>
     <t>ACABADOS DE PISOS</t>
   </si>
   <si>
-    <t>sdsd</t>
-  </si>
-  <si>
-    <t>FE.01.022</t>
-  </si>
-  <si>
-    <t>CIELO RASO PVC BLANCO TIPO DUELA 5.7 X 0.2 M</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ADOQUINADO</t>
+  </si>
+  <si>
+    <t>BAJA DESPERDICIOS</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>FE.01.001</t>
+  </si>
+  <si>
+    <t>AREAS  VERDES Y RECREATIVAS</t>
+  </si>
+  <si>
+    <t>FE.27.002</t>
+  </si>
+  <si>
+    <t>CLAVOS 2 1/2" X 10</t>
+  </si>
+  <si>
+    <t>CADENAS,CANDADOS,CLAVOS</t>
+  </si>
+  <si>
+    <t>BAJA NO CALIDAD</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -306,7 +330,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -627,22 +651,23 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:AZ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="52.987061" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="35.2771" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="32.991943" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="32.991943" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9.10" bestFit="true" style="0"/>
+    <col min="8" max="8" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="9.10" bestFit="true" style="0"/>
     <col min="52" max="52" width="9.10" bestFit="true" style="0"/>
     <col min="1" max="1" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -673,7 +698,8 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="2"/>
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">
@@ -701,7 +727,7 @@
               <sz val="8"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">23:51
+            <t xml:space="preserve">21:53
 </t>
           </r>
           <r>
@@ -726,7 +752,7 @@
               <sz val="8"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">01-09-2020
+            <t xml:space="preserve">07-10-2020
 </t>
           </r>
           <r>
@@ -781,19 +807,22 @@
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="C3" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="D3">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>13</v>
@@ -801,67 +830,99 @@
       <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:52">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:52">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
-      </c>
-      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:52">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>